<commit_message>
Centralizar a notificacao de progresso
</commit_message>
<xml_diff>
--- a/errors/template_errors.xlsx
+++ b/errors/template_errors.xlsx
@@ -402,12 +402,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>DSD: HTS_TST (Facility)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>2022-08-31 TEMPLATE ERROR ('MER C&amp;T|MER_ATS_Xipamanine_12'): O ficheiro de importacao nao esta consistente, a cellula: A5 Devia ter o valor: 'DSD: TX_NEW'</t>
         </is>
       </c>
     </row>
@@ -429,12 +429,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>Subtotal</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>2022-08-31 TEMPLATE ERROR ('MER C&amp;T|MER_ATS_Xipamanine_12'): O ficheiro de importacao nao esta consistente, a cellula: A21 Devia ter o valor: 'DSD: TX_CURR'</t>
         </is>
       </c>
     </row>
@@ -456,12 +456,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>2022-08-31 TEMPLATE ERROR ('MER C&amp;T|MER_ATS_Xipamanine_12'): O ficheiro de importacao nao esta consistente, a cellula: A44 Devia ter o valor: 'DSD: TX_RTT'</t>
         </is>
       </c>
     </row>
@@ -483,12 +483,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>Subtotal</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>2022-08-31 TEMPLATE ERROR ('MER C&amp;T|MER_ATS_Xipamanine_12'): O ficheiro de importacao nao esta consistente, a cellula: A62 Devia ter o valor: 'DSD: TX_ML'</t>
         </is>
       </c>
     </row>
@@ -510,12 +510,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>2022-08-31 TEMPLATE ERROR ('MER C&amp;T|MER_ATS_Xipamanine_12'): O ficheiro de importacao nao esta consistente, a cellula: A99 Devia ter o valor: 'DSD: PMTCT_ART'</t>
         </is>
       </c>
     </row>
@@ -535,14 +535,9 @@
           <t>DSD: TX_PVLS (Numerator)</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>DSD: TX_PVLS (Numerator) 34</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-08-30 TEMPLATE ERROR ('MER C&amp;T|MER_CT_1Junho_8'): O ficheiro de importacao nao esta consistente, a cellula: A114 Devia ter o valor: 'DSD: TX_PVLS (Numerator)'</t>
+          <t>2022-08-31 TEMPLATE ERROR ('MER C&amp;T|MER_ATS_Xipamanine_12'): O ficheiro de importacao nao esta consistente, a cellula: A114 Devia ter o valor: 'DSD: TX_PVLS (Numerator)'</t>
         </is>
       </c>
     </row>
@@ -564,12 +559,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>2022-08-31 TEMPLATE ERROR ('MER C&amp;T|MER_ATS_Xipamanine_12'): O ficheiro de importacao nao esta consistente, a cellula: A134 Devia ter o valor: 'DSD:TX_PVLS (Denominator)'</t>
         </is>
       </c>
     </row>
@@ -591,12 +586,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>Auto-Calculate</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>2022-08-31 TEMPLATE ERROR ('MER C&amp;T|MER_ATS_Xipamanine_12'): O ficheiro de importacao nao esta consistente, a cellula: A164 Devia ter o valor: 'DSD: TX_TB (Denominator)'</t>
         </is>
       </c>
     </row>
@@ -616,14 +611,9 @@
           <t>DSD: TB_ART (Numerator)</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>2022-08-31 TEMPLATE ERROR ('MER C&amp;T|MER_ATS_Xipamanine_12'): O ficheiro de importacao nao esta consistente, a cellula: A182 Devia ter o valor: 'DSD: TB_ART (Numerator)'</t>
         </is>
       </c>
     </row>

</xml_diff>